<commit_message>
Change rat's basis components labels to alphabetical order
</commit_message>
<xml_diff>
--- a/RunwayCombinationTable.xlsx
+++ b/RunwayCombinationTable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stakahas\Dropbox\github\reconfigurablemazeparts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stakahas\Documents\GitHub\ReconfigurableMazeParts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3E4305-8514-4A97-9A18-BBDD55EDD04D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284D145A-849E-41C9-8827-5D121E54EA8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17660" activeTab="1" xr2:uid="{D56FF8A7-3665-49A5-A2B8-FFFE452CD47E}"/>
   </bookViews>
@@ -175,26 +175,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>T,U,V</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C,F,G,H,I,J,K,L,V</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C,F,H,I,J,K,L,V</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C,Q,R,S,V</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C,W,X,V</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>A,B,C,D,G,H,I</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -260,6 +240,26 @@
   </si>
   <si>
     <t>Right and Left</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C,F,G,H,I,J,K,L,T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C,F,H,I,J,K,L,T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C,Q,R,S,T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C,U,V,T</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>W,X,T</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -646,10 +646,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -665,7 +665,7 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -673,7 +673,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -681,7 +681,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -689,12 +689,12 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -706,7 +706,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -874,7 +874,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -893,15 +893,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -909,31 +909,31 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -941,34 +941,34 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1070,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -1155,7 +1155,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1172,7 +1172,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1189,7 +1189,7 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -1223,7 +1223,7 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1240,7 +1240,7 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1257,7 +1257,7 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>5</v>
@@ -1274,7 +1274,7 @@
         <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1291,7 +1291,7 @@
         <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1322,7 +1322,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>2</v>

</xml_diff>